<commit_message>
The file template.xlsx was modified: The field with postal code was added.
</commit_message>
<xml_diff>
--- a/conf/templates/template.xlsx
+++ b/conf/templates/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Косых Евгений\Documents\eclipse-luna-workspace\ExportKvitReestr\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IdeaProjects\KvitMaker\conf\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Приложение №3</t>
   </si>
@@ -48,15 +48,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Итого квитанций в пачке:  </t>
   </si>
   <si>
@@ -73,6 +64,9 @@
   </si>
   <si>
     <t>&lt;IS_MKD&gt;</t>
+  </si>
+  <si>
+    <t>Почтовый индекс</t>
   </si>
 </sst>
 </file>
@@ -109,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -132,13 +126,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -162,6 +182,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -512,118 +544,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E14"/>
+  <dimension ref="B1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+      <selection activeCell="C10" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
     <col min="2" max="2" width="66.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="256" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="257" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E2" s="1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-    </row>
-    <row r="10" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="10" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="F14" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B6:E6"/>
+  <mergeCells count="6">
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>